<commit_message>
Enhance Staff Management, QR Security, Fix Build
</commit_message>
<xml_diff>
--- a/public/template_import_orders.xlsx
+++ b/public/template_import_orders.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project Code Kiem Tien\Rip egfulfill Jack NG\egfulfill-clone\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project Code Kiem Tien\Rip egfulfill Jack NG\egfulfill-clone\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BDD9F75-E063-427A-8D89-75BBA2A675DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4970A8C-0155-4A08-A699-4FF069E977EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6495" yWindow="3360" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="46">
   <si>
     <t>ORDER ID</t>
   </si>
@@ -109,13 +109,7 @@
     <t>BLACK</t>
   </si>
   <si>
-    <t>5XL</t>
-  </si>
-  <si>
     <t>Eva</t>
-  </si>
-  <si>
-    <t>3028 Stratford Court, Raleigh, North Carolina, 27604</t>
   </si>
   <si>
     <t>note</t>
@@ -128,27 +122,6 @@
   </si>
   <si>
     <t>EMBROIDERY</t>
-  </si>
-  <si>
-    <t>HOODIE-PREM</t>
-  </si>
-  <si>
-    <t>TSHIRT-BASIC</t>
-  </si>
-  <si>
-    <t>WHITE</t>
-  </si>
-  <si>
-    <t>XL</t>
-  </si>
-  <si>
-    <t>Henry</t>
-  </si>
-  <si>
-    <t>557 wtf street, California, USA, 7393</t>
-  </si>
-  <si>
-    <t>wataonima</t>
   </si>
   <si>
     <t>cho anh xin 2 vi</t>
@@ -170,6 +143,24 @@
   </si>
   <si>
     <t>ORDER2030</t>
+  </si>
+  <si>
+    <t>EM-18500</t>
+  </si>
+  <si>
+    <t>2XL</t>
+  </si>
+  <si>
+    <t>EM-1048-BOYMOM</t>
+  </si>
+  <si>
+    <t>RED</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>2165 E 41 Ave, Vancouver, BC Canada, V5P 1L3</t>
   </si>
 </sst>
 </file>
@@ -817,7 +808,7 @@
   <dimension ref="A1:AA1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -933,10 +924,10 @@
     </row>
     <row r="2" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C2" s="10">
         <v>2</v>
@@ -945,31 +936,31 @@
         <v>27</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G2" s="10"/>
       <c r="H2" s="10" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
       <c r="K2" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="L2" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="M2" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="L2" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="M2" s="11" t="s">
-        <v>33</v>
-      </c>
       <c r="N2" s="11" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="O2" s="10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="P2" s="10"/>
       <c r="Q2" s="12"/>
@@ -986,51 +977,49 @@
     </row>
     <row r="3" spans="1:27" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C3" s="10">
         <v>1</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="G3" s="10"/>
       <c r="H3" s="10" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
-      <c r="I3" s="10" t="s">
-        <v>41</v>
-      </c>
+      <c r="I3" s="10"/>
       <c r="J3" s="10"/>
       <c r="K3" s="10" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="L3" s="10" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="M3" s="15" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="N3" s="16" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="O3" s="10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="P3" s="10" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="Q3" s="10" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="R3" s="10"/>
       <c r="S3" s="10"/>

</xml_diff>